<commit_message>
feat(network): select the network
</commit_message>
<xml_diff>
--- a/docs/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/docs/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\joachim-MonProjetGenial\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D449E3-5C88-4D41-8424-CC9011B56445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C9F47C-8F05-4DA7-ABB9-E4072E124EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -132,6 +132,18 @@
   </si>
   <si>
     <t>Écouter les instructions et les décisions sur les enveloppes</t>
+  </si>
+  <si>
+    <t>Je voulais vérifier que j'étais bien connecté au Broker mais il ne tourne pas actuellement, j'essayerai de me connecter au blue plus tard, je code l'interface utilisateur.</t>
+  </si>
+  <si>
+    <t>Je me connecte au broker blue, j'ai trouvé l'adresse IP du broker depuis un repo créé spécialement par Philippe</t>
+  </si>
+  <si>
+    <t>Je crée des radioBox et j'essaie de changer le BrokerIP selon ce qui est sélectionné.</t>
+  </si>
+  <si>
+    <t>Changement du BrokerIP selon le réseau sélectionné.</t>
   </si>
 </sst>
 </file>
@@ -643,7 +655,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -711,7 +723,7 @@
       </c>
       <c r="C3" s="25">
         <f>SUM(C6:C521)</f>
-        <v>0.22569444444444442</v>
+        <v>0.29861111111111105</v>
       </c>
       <c r="D3" s="29" t="s">
         <v>13</v>
@@ -952,48 +964,80 @@
       </c>
       <c r="F16" s="10"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="str">
+    <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="20"/>
+        <v>48</v>
+      </c>
+      <c r="B17" s="8">
+        <v>45625</v>
+      </c>
+      <c r="C17" s="24">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>31</v>
+      </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="str">
+    <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="10"/>
+        <v>48</v>
+      </c>
+      <c r="B18" s="8">
+        <v>45625</v>
+      </c>
+      <c r="C18" s="24">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>32</v>
+      </c>
       <c r="F18" s="10"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="str">
+      <c r="A19" s="13">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="10"/>
+        <v>48</v>
+      </c>
+      <c r="B19" s="8">
+        <v>45625</v>
+      </c>
+      <c r="C19" s="24">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="F19" s="10"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="str">
+      <c r="A20" s="13">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="20"/>
+        <v>48</v>
+      </c>
+      <c r="B20" s="8">
+        <v>45625</v>
+      </c>
+      <c r="C20" s="24">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>34</v>
+      </c>
       <c r="F20" s="22"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
chore(work diary): update work diary
</commit_message>
<xml_diff>
--- a/docs/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/docs/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\joachim-MonProjetGenial\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3D3610-03BB-4E10-A87F-8DE18E41F438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0E46BB-0A32-4319-A8D4-1C9871204551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -664,7 +664,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -732,7 +732,7 @@
       </c>
       <c r="C3" s="25">
         <f>SUM(C6:C521)</f>
-        <v>0.34027777777777768</v>
+        <v>0.35069444444444436</v>
       </c>
       <c r="D3" s="29" t="s">
         <v>13</v>
@@ -1096,7 +1096,7 @@
         <v>45625</v>
       </c>
       <c r="C23" s="24">
-        <v>6.9444444444444441E-3</v>
+        <v>1.7361111111111112E-2</v>
       </c>
       <c r="D23" s="21" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
refactor(MQTT connection): change connection
30m-DONE-#2
</commit_message>
<xml_diff>
--- a/docs/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/docs/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\joachim-MonProjetGenial\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0E46BB-0A32-4319-A8D4-1C9871204551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8222604E-17BA-42E1-8FE6-7883E9FAFB63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Je récupère les informations nécessaires de mon fichier.</t>
+  </si>
+  <si>
+    <t>J'affiche les fichiers dans ma bibliothèque (sans connexion au MQTT)</t>
   </si>
 </sst>
 </file>
@@ -664,7 +667,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -732,7 +735,7 @@
       </c>
       <c r="C3" s="25">
         <f>SUM(C6:C521)</f>
-        <v>0.35069444444444436</v>
+        <v>0.38194444444444436</v>
       </c>
       <c r="D3" s="29" t="s">
         <v>13</v>
@@ -1107,14 +1110,22 @@
       <c r="F23" s="10"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="str">
+      <c r="A24" s="13">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="10"/>
+        <v>50</v>
+      </c>
+      <c r="B24" s="8">
+        <v>45639</v>
+      </c>
+      <c r="C24" s="24">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="F24" s="10"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -6736,6 +6747,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -6958,27 +6989,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6995,23 +7025,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
chore(documentation): add the documentation
</commit_message>
<xml_diff>
--- a/docs/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/docs/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\joachim-MonProjetGenial\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8222604E-17BA-42E1-8FE6-7883E9FAFB63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB8093E-DF93-4A28-822F-446B7AB12C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -156,6 +156,24 @@
   </si>
   <si>
     <t>J'affiche les fichiers dans ma bibliothèque (sans connexion au MQTT)</t>
+  </si>
+  <si>
+    <t>Je me connecte au broker blue avec les options donnés dans le README créé par Philippe, j'ai dû modifié un peu le code donc ça m'a pris plus de temps.</t>
+  </si>
+  <si>
+    <t>Je règle une erreur qui faisait crash mon code et je continue la création de mon menu pour chercher les catalogues (la recherche MQTT se fera après)</t>
+  </si>
+  <si>
+    <t>Évaluation des ~80%</t>
+  </si>
+  <si>
+    <t>J'ai un cours à rattraper</t>
+  </si>
+  <si>
+    <t>J'essaie d'implémenter le code fourni pour MQTT, je n'arrive pas à comprendre la logique des enveloppes.</t>
+  </si>
+  <si>
+    <t>Je crée la base du rapport</t>
   </si>
 </sst>
 </file>
@@ -455,6 +473,61 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3143250</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>6051843</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38224</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEBB1963-9FD0-1FB5-EC68-18CCB23233A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13487400" y="6553200"/>
+          <a:ext cx="2908593" cy="619249"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45CB4986-052B-374B-A8D0-88D41B362A09}" name="Table2" displayName="Table2" ref="A5:F531" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A5:F531" xr:uid="{45CB4986-052B-374B-A8D0-88D41B362A09}">
@@ -666,8 +739,8 @@
   <dimension ref="A1:N531"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+      <pane ySplit="5" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -735,7 +808,7 @@
       </c>
       <c r="C3" s="25">
         <f>SUM(C6:C521)</f>
-        <v>0.38194444444444436</v>
+        <v>0.47569444444444436</v>
       </c>
       <c r="D3" s="29" t="s">
         <v>13</v>
@@ -1128,59 +1201,101 @@
       </c>
       <c r="F24" s="10"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="str">
+    <row r="25" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="13">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="10"/>
+        <v>50</v>
+      </c>
+      <c r="B25" s="8">
+        <v>45639</v>
+      </c>
+      <c r="C25" s="24">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>39</v>
+      </c>
       <c r="F25" s="10"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="str">
+    <row r="26" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
         <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="10"/>
+        <v>50</v>
+      </c>
+      <c r="B26" s="8">
+        <v>45639</v>
+      </c>
+      <c r="C26" s="24">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>40</v>
+      </c>
       <c r="F26" s="10"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="str">
+      <c r="A27" s="13">
         <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="10"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="str">
+        <v>50</v>
+      </c>
+      <c r="B27" s="8">
+        <v>45639</v>
+      </c>
+      <c r="C27" s="24">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
         <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="20"/>
+        <v>50</v>
+      </c>
+      <c r="B28" s="8">
+        <v>45639</v>
+      </c>
+      <c r="C28" s="24">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="F28" s="22"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="str">
+      <c r="A29" s="13">
         <f>IF(ISBLANK(B29),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="20"/>
+        <v>50</v>
+      </c>
+      <c r="B29" s="8">
+        <v>45639</v>
+      </c>
+      <c r="C29" s="24">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>44</v>
+      </c>
       <c r="F29" s="10"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -6740,8 +6855,9 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
feat(MQTT): Listen for catalog asking and answer them
</commit_message>
<xml_diff>
--- a/docs/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/docs/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\joachim-MonProjetGenial\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB8093E-DF93-4A28-822F-446B7AB12C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97288EC-5151-4A68-9888-96D139874FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>Je crée la base du rapport</t>
+  </si>
+  <si>
+    <t>J'essaie de donner mon catalogue quand on me le demande. J'arrive à répondre un message il faut juste que le message soit mon catalogue. J'ai réussi à l'envoyer et à le recevoir. J'ai trouvé quand faire appel à la fonction.</t>
   </si>
 </sst>
 </file>
@@ -478,15 +481,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>3143250</xdr:colOff>
+      <xdr:colOff>3154456</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>234763</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>6051843</xdr:colOff>
+      <xdr:colOff>6063049</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>38224</xdr:rowOff>
+      <xdr:rowOff>253937</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -515,8 +518,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13487400" y="6553200"/>
-          <a:ext cx="2908593" cy="619249"/>
+          <a:off x="13497485" y="6750984"/>
+          <a:ext cx="2908593" cy="618688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -739,8 +742,8 @@
   <dimension ref="A1:N531"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
+      <pane ySplit="5" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -808,7 +811,7 @@
       </c>
       <c r="C3" s="25">
         <f>SUM(C6:C521)</f>
-        <v>0.47569444444444436</v>
+        <v>0.52083333333333326</v>
       </c>
       <c r="D3" s="29" t="s">
         <v>13</v>
@@ -1298,15 +1301,23 @@
       </c>
       <c r="F29" s="10"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="str">
+    <row r="30" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="13">
         <f>IF(ISBLANK(B30),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="10"/>
+        <v>51</v>
+      </c>
+      <c r="B30" s="8">
+        <v>45646</v>
+      </c>
+      <c r="C30" s="24">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>45</v>
+      </c>
       <c r="F30" s="10"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -6863,26 +6874,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -7105,26 +7096,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7141,4 +7133,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
docs(documentation): add introduction and analyse
50m-WIP-#12
</commit_message>
<xml_diff>
--- a/docs/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/docs/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\joachim-MonProjetGenial\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97288EC-5151-4A68-9888-96D139874FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28582EDB-063F-4DBC-B0FF-D829D1E3AC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>Mise en place du rapport/journal de travail</t>
-  </si>
-  <si>
-    <t>Création de la planification</t>
   </si>
   <si>
     <t>Réunion pour définir le programme de la journée. Et analyser le code Rust de génération automatique du journal de travail.</t>
@@ -177,6 +174,18 @@
   </si>
   <si>
     <t>J'essaie de donner mon catalogue quand on me le demande. J'arrive à répondre un message il faut juste que le message soit mon catalogue. J'ai réussi à l'envoyer et à le recevoir. J'ai trouvé quand faire appel à la fonction.</t>
+  </si>
+  <si>
+    <t>Répondre à une entreprise</t>
+  </si>
+  <si>
+    <t>Création de la planification et des maquettes</t>
+  </si>
+  <si>
+    <t>Selon l'évaluation des 80% je rajoute des détails techniques sur mes maquettes</t>
+  </si>
+  <si>
+    <t>J'avance sur le rapport, reporter les maquettes, faire l'introduction.</t>
   </si>
 </sst>
 </file>
@@ -743,7 +752,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -811,7 +820,7 @@
       </c>
       <c r="C3" s="25">
         <f>SUM(C6:C521)</f>
-        <v>0.52083333333333326</v>
+        <v>0.54513888888888873</v>
       </c>
       <c r="D3" s="29" t="s">
         <v>13</v>
@@ -896,7 +905,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="F8" s="23"/>
     </row>
@@ -915,7 +924,7 @@
         <v>11</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="10"/>
     </row>
@@ -934,7 +943,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" s="22"/>
     </row>
@@ -953,7 +962,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11" s="10"/>
     </row>
@@ -972,7 +981,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" s="10"/>
     </row>
@@ -991,7 +1000,7 @@
         <v>17</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13" s="10"/>
     </row>
@@ -1010,7 +1019,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" s="10"/>
     </row>
@@ -1029,7 +1038,7 @@
         <v>8</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15" s="10"/>
     </row>
@@ -1048,7 +1057,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F16" s="10"/>
     </row>
@@ -1067,7 +1076,7 @@
         <v>8</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F17" s="22"/>
     </row>
@@ -1086,7 +1095,7 @@
         <v>8</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F18" s="10"/>
     </row>
@@ -1105,7 +1114,7 @@
         <v>8</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F19" s="10"/>
     </row>
@@ -1124,7 +1133,7 @@
         <v>8</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F20" s="22"/>
     </row>
@@ -1143,7 +1152,7 @@
         <v>8</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F21" s="10"/>
     </row>
@@ -1162,7 +1171,7 @@
         <v>8</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F22" s="22"/>
     </row>
@@ -1181,7 +1190,7 @@
         <v>8</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F23" s="10"/>
     </row>
@@ -1200,7 +1209,7 @@
         <v>8</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F24" s="10"/>
     </row>
@@ -1219,7 +1228,7 @@
         <v>8</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F25" s="10"/>
     </row>
@@ -1238,7 +1247,7 @@
         <v>8</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F26" s="10"/>
     </row>
@@ -1257,10 +1266,10 @@
         <v>11</v>
       </c>
       <c r="E27" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
@@ -1278,7 +1287,7 @@
         <v>8</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F28" s="22"/>
     </row>
@@ -1297,7 +1306,7 @@
         <v>10</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F29" s="10"/>
     </row>
@@ -1316,41 +1325,65 @@
         <v>8</v>
       </c>
       <c r="E30" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" s="10"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="13">
+        <f>IF(ISBLANK(B31),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
+        <v>51</v>
+      </c>
+      <c r="B31" s="8">
+        <v>45646</v>
+      </c>
+      <c r="C31" s="24">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F30" s="10"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="str">
-        <f>IF(ISBLANK(B31),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="10"/>
       <c r="F31" s="10"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="str">
+      <c r="A32" s="13">
         <f>IF(ISBLANK(B32),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="10"/>
+        <v>51</v>
+      </c>
+      <c r="B32" s="8">
+        <v>45646</v>
+      </c>
+      <c r="C32" s="24">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="D32" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>47</v>
+      </c>
       <c r="F32" s="10"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="str">
+      <c r="A33" s="13">
         <f>IF(ISBLANK(B33),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="10"/>
+        <v>51</v>
+      </c>
+      <c r="B33" s="8">
+        <v>45646</v>
+      </c>
+      <c r="C33" s="24">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>48</v>
+      </c>
       <c r="F33" s="10"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat(envelope): add missing messageType, rename them
</commit_message>
<xml_diff>
--- a/docs/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/docs/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\joachim-MonProjetGenial\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28582EDB-063F-4DBC-B0FF-D829D1E3AC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1576AA72-5F8F-4C3B-9648-C633A017DBE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -752,7 +752,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -820,7 +820,7 @@
       </c>
       <c r="C3" s="25">
         <f>SUM(C6:C521)</f>
-        <v>0.54513888888888873</v>
+        <v>0.54166666666666652</v>
       </c>
       <c r="D3" s="29" t="s">
         <v>13</v>
@@ -1376,7 +1376,7 @@
         <v>45646</v>
       </c>
       <c r="C33" s="24">
-        <v>1.0416666666666666E-2</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="D33" s="21" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
feat(MQTT send catalog): advance in my catalog
40m-WIP
</commit_message>
<xml_diff>
--- a/docs/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/docs/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\joachim-MonProjetGenial\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8612DF-F08E-4AB0-B91D-FA0DAF296A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBC0D6C-83A6-4D8A-9CB0-FDE5B4050810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>Au clic bouton "Rechercher" une demande de catalogue est envoyé, testé avec Tiago cela fonctionne.</t>
+  </si>
+  <si>
+    <t>J'avance sur donner mon catalogue</t>
   </si>
 </sst>
 </file>
@@ -758,7 +761,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -826,7 +829,7 @@
       </c>
       <c r="C3" s="25">
         <f>SUM(C6:C521)</f>
-        <v>0.61805555555555547</v>
+        <v>0.64583333333333326</v>
       </c>
       <c r="D3" s="29" t="s">
         <v>13</v>
@@ -1431,14 +1434,22 @@
       <c r="F35" s="10"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="str">
+      <c r="A36" s="13">
         <f>IF(ISBLANK(B36),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="10"/>
+        <v>51</v>
+      </c>
+      <c r="B36" s="8">
+        <v>45646</v>
+      </c>
+      <c r="C36" s="24">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="F36" s="10"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
docs: update work diary and documentation
</commit_message>
<xml_diff>
--- a/docs/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/docs/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyco\Documents\GitHub\joachim-MonProjetGenial\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CF9EB2-6369-4632-A299-010BB8A6EBF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D0DC50-ED7F-4FD3-81B1-47F2A808FEDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>Je duplique mon projet et je simule 2 clients, mon application fonctionne. Cela fonctionne donc avec toutes les personnes ayant suivi les normes d'enveloppes proposés dans le GitHub de Philippe.</t>
+  </si>
+  <si>
+    <t>Je termine mon rapport</t>
   </si>
 </sst>
 </file>
@@ -792,7 +795,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
+      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -860,7 +863,7 @@
       </c>
       <c r="C3" s="25">
         <f>SUM(C6:C521)</f>
-        <v>0.86805555555555536</v>
+        <v>0.8819444444444442</v>
       </c>
       <c r="D3" s="29" t="s">
         <v>13</v>
@@ -1674,14 +1677,22 @@
       <c r="F46" s="20"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="13" t="str">
+      <c r="A47" s="13">
         <f>IF(ISBLANK(B47),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="10"/>
+        <v>2</v>
+      </c>
+      <c r="B47" s="8">
+        <v>45668</v>
+      </c>
+      <c r="C47" s="24">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="D47" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>62</v>
+      </c>
       <c r="F47" s="10"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
@@ -7060,6 +7071,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -7282,17 +7304,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
   <ds:schemaRefs>
@@ -7302,6 +7313,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7318,15 +7340,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>